<commit_message>
update UMo rad damage
</commit_message>
<xml_diff>
--- a/USHPRR/UMo_radiation_damage.xlsx
+++ b/USHPRR/UMo_radiation_damage.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beelbw/projects/spreadsheets/USHPRR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminbeeler/projects/spreadsheets/USHPRR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF519BCB-83B9-2548-B876-06F90B10B83C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A35042-7183-374C-8F01-999CDAEC68BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18940" yWindow="3480" windowWidth="27240" windowHeight="16440" xr2:uid="{6147F9BE-C613-5E42-8D18-16DEAC3FC724}"/>
+    <workbookView xWindow="1000" yWindow="1060" windowWidth="27240" windowHeight="16440" xr2:uid="{6147F9BE-C613-5E42-8D18-16DEAC3FC724}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -4305,8 +4305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3A0157-F4A1-D343-9CE3-032F57D3E6BB}">
   <dimension ref="B1:X55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AA3" sqref="AA3"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>